<commit_message>
add fall foliage graphics submitted by renratpiz
</commit_message>
<xml_diff>
--- a/resource/textures/texture-index.xlsx
+++ b/resource/textures/texture-index.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="texture_index" localSheetId="0">Sheet1!$A$1:$B$1404</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="1404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="1411">
   <si>
     <t>Brick Blue</t>
   </si>
@@ -4244,6 +4245,27 @@
   </si>
   <si>
     <t>jala - fance</t>
+  </si>
+  <si>
+    <t>fall leaves 1 replaces #9606</t>
+  </si>
+  <si>
+    <t>fall leaves 2 replaces #9605</t>
+  </si>
+  <si>
+    <t>fall leaves 3 replaces #1503</t>
+  </si>
+  <si>
+    <t>fall leaves 4 replaces #1502</t>
+  </si>
+  <si>
+    <t>fall leaves 5 replaces #1501</t>
+  </si>
+  <si>
+    <t>fall leaves 6 replaces #9608</t>
+  </si>
+  <si>
+    <t>fall leaves 7 replaces #9777 and #10001</t>
   </si>
 </sst>
 </file>
@@ -4290,8 +4312,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4591,10 +4641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1421"/>
+  <dimension ref="A1:B1428"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1403" workbookViewId="0">
-      <selection activeCell="D1371" sqref="D1371"/>
+      <selection activeCell="B1429" sqref="B1429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15969,6 +16019,62 @@
       </c>
       <c r="B1421" s="1" t="s">
         <v>1373</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1422" s="2">
+        <v>61018</v>
+      </c>
+      <c r="B1422" s="1" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1423" s="2">
+        <v>61019</v>
+      </c>
+      <c r="B1423" s="1" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1424" s="2">
+        <v>61020</v>
+      </c>
+      <c r="B1424" s="1" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1425" s="2">
+        <v>61021</v>
+      </c>
+      <c r="B1425" s="1" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1426" s="2">
+        <v>61022</v>
+      </c>
+      <c r="B1426" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1427" s="2">
+        <v>61023</v>
+      </c>
+      <c r="B1427" s="1" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1428" s="2">
+        <v>61024</v>
+      </c>
+      <c r="B1428" s="1" t="s">
+        <v>1410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional fall textures from renratpiz
</commit_message>
<xml_diff>
--- a/resource/textures/texture-index.xlsx
+++ b/resource/textures/texture-index.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="1411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="1418">
   <si>
     <t>Brick Blue</t>
   </si>
@@ -4266,6 +4266,27 @@
   </si>
   <si>
     <t>fall leaves 7 replaces #9777 and #10001</t>
+  </si>
+  <si>
+    <t>fall leaves 8 replaces #8866</t>
+  </si>
+  <si>
+    <t>fall leaves 9 replaces #8865</t>
+  </si>
+  <si>
+    <t>fall leaves 10 replaces #9766 and #10000</t>
+  </si>
+  <si>
+    <t>fall leaves 11 replaces #8861</t>
+  </si>
+  <si>
+    <t>fall leaves 12 replaces #8862</t>
+  </si>
+  <si>
+    <t>fall leaves 13 replaces #8863</t>
+  </si>
+  <si>
+    <t>fall leaves 14 replaces #8864</t>
   </si>
 </sst>
 </file>
@@ -4641,10 +4662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1428"/>
+  <dimension ref="A1:B1435"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1403" workbookViewId="0">
-      <selection activeCell="B1429" sqref="B1429"/>
+      <selection activeCell="B1436" sqref="B1436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16075,6 +16096,62 @@
       </c>
       <c r="B1428" s="1" t="s">
         <v>1410</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1429" s="2">
+        <v>61025</v>
+      </c>
+      <c r="B1429" s="1" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1430" s="2">
+        <v>61026</v>
+      </c>
+      <c r="B1430" s="1" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1431" s="2">
+        <v>61027</v>
+      </c>
+      <c r="B1431" s="1" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1432" s="2">
+        <v>61028</v>
+      </c>
+      <c r="B1432" s="1" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1433" s="2">
+        <v>61029</v>
+      </c>
+      <c r="B1433" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1434" s="2">
+        <v>61030</v>
+      </c>
+      <c r="B1434" s="1" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1435" s="2">
+        <v>61031</v>
+      </c>
+      <c r="B1435" s="1" t="s">
+        <v>1417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>